<commit_message>
Adde excel and Test
</commit_message>
<xml_diff>
--- a/KasimMavenProject/src/test/resources/excel/TestDataExcel.xlsx
+++ b/KasimMavenProject/src/test/resources/excel/TestDataExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vn06185/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA3DE1F-6CB0-D44F-B903-4CC42A034C2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D483D0C-C561-BE4B-8708-45E2DDFD90F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16700" activeTab="2" xr2:uid="{7969ACE7-1229-6042-B065-4B7AF7E51350}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -55,9 +55,6 @@
     <t>PostCode</t>
   </si>
   <si>
-    <t>sss</t>
-  </si>
-  <si>
     <t>CardNumber</t>
   </si>
   <si>
@@ -83,6 +80,24 @@
   </si>
   <si>
     <t>4811111111111113</t>
+  </si>
+  <si>
+    <t>Kasim</t>
+  </si>
+  <si>
+    <t>mdkasim111@hotmail.com</t>
+  </si>
+  <si>
+    <t>Jakarta</t>
+  </si>
+  <si>
+    <t>081808466410</t>
+  </si>
+  <si>
+    <t>MidPlaza 2, 4th Floor Jl.Jend.Sudirman Kav.10-11</t>
+  </si>
+  <si>
+    <t>10220</t>
   </si>
 </sst>
 </file>
@@ -435,13 +450,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA50D23-66BC-4848-98A8-2BD311FD64A1}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -463,9 +483,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F5" t="s">
-        <v>6</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -488,30 +523,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -524,7 +559,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,30 +569,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>